<commit_message>
Add percentStarted to roster parsing and auto-fill starters
Introduces a 'Percent Started' column to the Excel export and updates the TypeScript types and parser to support it. Bench players with the highest percentStarted values are now used to auto-fill missing starter slots when possible, improving roster completeness. Updates include changes to the Excel output, parser logic, and Player type definition.
</commit_message>
<xml_diff>
--- a/data/roster_dub.xlsx
+++ b/data/roster_dub.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F200"/>
+  <dimension ref="A1:G200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,6 +452,11 @@
           <t>Injury Status</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Percent Started</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -484,6 +489,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G2" t="n">
+        <v>95.58</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -516,6 +524,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G3" t="n">
+        <v>95.89</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -548,6 +559,9 @@
           <t>INJURY_RESERVE</t>
         </is>
       </c>
+      <c r="G4" t="n">
+        <v>8.17</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -580,6 +594,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G5" t="n">
+        <v>15.93</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -612,6 +629,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G6" t="n">
+        <v>42.59</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -644,6 +664,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G7" t="n">
+        <v>98.36</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -676,6 +699,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G8" t="n">
+        <v>6.43</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -708,6 +734,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G9" t="n">
+        <v>38.23</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -740,6 +769,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G10" t="n">
+        <v>74.62</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -772,6 +804,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G11" t="n">
+        <v>51.58</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -804,6 +839,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G12" t="n">
+        <v>61.47</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -836,6 +874,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G13" t="n">
+        <v>26.17</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -868,6 +909,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G14" t="n">
+        <v>30.26</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -900,6 +944,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G15" t="n">
+        <v>1.22</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -932,6 +979,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G16" t="n">
+        <v>43.75</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -964,6 +1014,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G17" t="n">
+        <v>26.03</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -996,6 +1049,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G18" t="n">
+        <v>15.08</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1028,6 +1084,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G19" t="n">
+        <v>98.97</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1060,6 +1119,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G20" t="n">
+        <v>42.75</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1092,6 +1154,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G21" t="n">
+        <v>47.36</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1124,6 +1189,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G22" t="n">
+        <v>75.58</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1156,6 +1224,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G23" t="n">
+        <v>23.08</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1188,6 +1259,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G24" t="n">
+        <v>46.18</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1220,6 +1294,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G25" t="n">
+        <v>34.89</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1252,6 +1329,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G26" t="n">
+        <v>21.61</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1284,6 +1364,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G27" t="n">
+        <v>27.72</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1316,6 +1399,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G28" t="n">
+        <v>2.02</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1348,6 +1434,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G29" t="n">
+        <v>94.13</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1380,6 +1469,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G30" t="n">
+        <v>12.65</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1412,6 +1504,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G31" t="n">
+        <v>12.29</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1444,6 +1539,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G32" t="n">
+        <v>62.69</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1476,6 +1574,9 @@
           <t>OUT</t>
         </is>
       </c>
+      <c r="G33" t="n">
+        <v>32.52</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1508,6 +1609,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G34" t="n">
+        <v>26.68</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1540,6 +1644,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G35" t="n">
+        <v>17.63</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1572,6 +1679,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G36" t="n">
+        <v>99.31999999999999</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1604,6 +1714,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G37" t="n">
+        <v>86.56</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1636,6 +1749,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G38" t="n">
+        <v>37.6</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1668,6 +1784,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G39" t="n">
+        <v>36.5</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1700,6 +1819,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G40" t="n">
+        <v>84.01000000000001</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1732,6 +1854,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G41" t="n">
+        <v>73.42</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1764,6 +1889,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G42" t="n">
+        <v>41.17</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1796,6 +1924,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G43" t="n">
+        <v>7.65</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1828,6 +1959,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G44" t="n">
+        <v>9.369999999999999</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1860,6 +1994,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G45" t="n">
+        <v>24.87</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1892,6 +2029,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G46" t="n">
+        <v>36.12</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1924,6 +2064,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G47" t="n">
+        <v>57.76</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1956,6 +2099,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G48" t="n">
+        <v>18.18</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1988,6 +2134,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G49" t="n">
+        <v>72.56</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2020,6 +2169,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G50" t="n">
+        <v>24.1</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2052,6 +2204,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G51" t="n">
+        <v>30.53</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2084,6 +2239,9 @@
           <t>INJURY_RESERVE</t>
         </is>
       </c>
+      <c r="G52" t="n">
+        <v>12.2</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2116,6 +2274,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G53" t="n">
+        <v>69.31</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2148,6 +2309,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G54" t="n">
+        <v>56.63</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2180,6 +2344,9 @@
           <t>INJURY_RESERVE</t>
         </is>
       </c>
+      <c r="G55" t="n">
+        <v>0.28</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2212,6 +2379,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G56" t="n">
+        <v>74.03</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2244,6 +2414,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G57" t="n">
+        <v>42.78</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2276,6 +2449,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G58" t="n">
+        <v>26.06</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2308,6 +2484,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G59" t="n">
+        <v>43.17</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2340,6 +2519,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G60" t="n">
+        <v>43.01</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2372,6 +2554,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G61" t="n">
+        <v>48.05</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2404,6 +2589,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G62" t="n">
+        <v>78.38</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2436,6 +2624,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G63" t="n">
+        <v>9.619999999999999</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2468,6 +2659,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G64" t="n">
+        <v>3.67</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2500,6 +2694,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G65" t="n">
+        <v>53.84</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2532,6 +2729,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G66" t="n">
+        <v>7.69</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2564,6 +2764,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G67" t="n">
+        <v>40.95</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2596,6 +2799,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G68" t="n">
+        <v>4.43</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2628,6 +2834,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G69" t="n">
+        <v>64.36</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2660,6 +2869,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G70" t="n">
+        <v>16.43</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2692,6 +2904,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G71" t="n">
+        <v>83.01000000000001</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2724,6 +2939,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G72" t="n">
+        <v>52.64</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2756,6 +2974,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G73" t="n">
+        <v>72.66</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2788,6 +3009,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G74" t="n">
+        <v>72.13</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2820,6 +3044,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G75" t="n">
+        <v>49.4</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2852,6 +3079,9 @@
           <t>INJURY_RESERVE</t>
         </is>
       </c>
+      <c r="G76" t="n">
+        <v>28.32</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2884,6 +3114,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G77" t="n">
+        <v>91.73</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2916,6 +3149,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G78" t="n">
+        <v>37.19</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2948,6 +3184,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G79" t="n">
+        <v>41.6</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2980,6 +3219,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G80" t="n">
+        <v>70.70999999999999</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3012,6 +3254,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G81" t="n">
+        <v>53.34</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3044,6 +3289,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G82" t="n">
+        <v>52.43</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3076,6 +3324,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G83" t="n">
+        <v>19.79</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3108,6 +3359,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G84" t="n">
+        <v>4.64</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3140,6 +3394,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G85" t="n">
+        <v>16.01</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3172,6 +3429,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G86" t="n">
+        <v>71.98999999999999</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3204,6 +3464,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G87" t="n">
+        <v>31.34</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3236,6 +3499,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G88" t="n">
+        <v>89.47</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3268,6 +3534,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G89" t="n">
+        <v>0.84</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3300,6 +3569,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G90" t="n">
+        <v>22.09</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3332,6 +3604,9 @@
           <t>OUT</t>
         </is>
       </c>
+      <c r="G91" t="n">
+        <v>0.08</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3364,6 +3639,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G92" t="n">
+        <v>24.59</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3396,6 +3674,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G93" t="n">
+        <v>94.02</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3428,6 +3709,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G94" t="n">
+        <v>8.02</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3460,6 +3744,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G95" t="n">
+        <v>55.49</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3492,6 +3779,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G96" t="n">
+        <v>17.87</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3524,6 +3814,9 @@
           <t>OUT</t>
         </is>
       </c>
+      <c r="G97" t="n">
+        <v>27.8</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3556,6 +3849,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G98" t="n">
+        <v>5.19</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3588,6 +3884,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G99" t="n">
+        <v>63.11</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3620,6 +3919,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G100" t="n">
+        <v>1.08</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3652,6 +3954,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G101" t="n">
+        <v>1.26</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3684,6 +3989,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G102" t="n">
+        <v>17.19</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3716,6 +4024,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G103" t="n">
+        <v>44.51</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3748,6 +4059,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G104" t="n">
+        <v>72.34999999999999</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3780,6 +4094,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G105" t="n">
+        <v>55.95</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3812,6 +4129,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G106" t="n">
+        <v>4.91</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3844,6 +4164,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G107" t="n">
+        <v>14.81</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3876,6 +4199,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G108" t="n">
+        <v>73.41</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3908,6 +4234,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G109" t="n">
+        <v>16.88</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3940,6 +4269,9 @@
           <t>INJURY_RESERVE</t>
         </is>
       </c>
+      <c r="G110" t="n">
+        <v>7.43</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -3972,6 +4304,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G111" t="n">
+        <v>64.79000000000001</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4004,6 +4339,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G112" t="n">
+        <v>18.9</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4036,6 +4374,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G113" t="n">
+        <v>46.18</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -4068,6 +4409,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G114" t="n">
+        <v>29.68</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4100,6 +4444,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G115" t="n">
+        <v>12.77</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -4132,6 +4479,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G116" t="n">
+        <v>66.97</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -4164,6 +4514,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G117" t="n">
+        <v>14.56</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -4196,6 +4549,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G118" t="n">
+        <v>37.99</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -4228,6 +4584,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G119" t="n">
+        <v>75.62</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -4260,6 +4619,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G120" t="n">
+        <v>94.44</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -4292,6 +4654,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G121" t="n">
+        <v>79.42</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -4324,6 +4689,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G122" t="n">
+        <v>24.1</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -4356,6 +4724,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G123" t="n">
+        <v>28.52</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -4388,6 +4759,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G124" t="n">
+        <v>14.37</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -4420,6 +4794,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G125" t="n">
+        <v>65.84</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -4452,6 +4829,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G126" t="n">
+        <v>58.82</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -4484,6 +4864,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G127" t="n">
+        <v>46.37</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -4516,6 +4899,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G128" t="n">
+        <v>68.52</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -4548,6 +4934,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G129" t="n">
+        <v>10.76</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -4580,6 +4969,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G130" t="n">
+        <v>13.5</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -4612,6 +5004,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G131" t="n">
+        <v>7.51</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -4644,6 +5039,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G132" t="n">
+        <v>20.73</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -4676,6 +5074,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G133" t="n">
+        <v>6.97</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -4708,6 +5109,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G134" t="n">
+        <v>30.39</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -4740,6 +5144,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G135" t="n">
+        <v>73.87</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -4772,6 +5179,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G136" t="n">
+        <v>61.65</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -4804,6 +5214,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G137" t="n">
+        <v>4.21</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -4836,6 +5249,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G138" t="n">
+        <v>82.40000000000001</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -4868,6 +5284,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G139" t="n">
+        <v>17.35</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -4900,6 +5319,9 @@
           <t>INJURY_RESERVE</t>
         </is>
       </c>
+      <c r="G140" t="n">
+        <v>0.51</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -4932,6 +5354,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G141" t="n">
+        <v>84.72</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -4964,6 +5389,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G142" t="n">
+        <v>0.6899999999999999</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -4996,6 +5424,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G143" t="n">
+        <v>70.01000000000001</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -5028,6 +5459,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G144" t="n">
+        <v>98.19</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -5060,6 +5494,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G145" t="n">
+        <v>86.02</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -5092,6 +5529,9 @@
           <t>OUT</t>
         </is>
       </c>
+      <c r="G146" t="n">
+        <v>1.31</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -5124,6 +5564,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G147" t="n">
+        <v>71.08</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -5156,6 +5599,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G148" t="n">
+        <v>1.71</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -5188,6 +5634,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G149" t="n">
+        <v>24.59</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -5220,6 +5669,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G150" t="n">
+        <v>0.86</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -5252,6 +5704,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G151" t="n">
+        <v>18.15</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -5284,6 +5739,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G152" t="n">
+        <v>99.59</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -5316,6 +5774,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G153" t="n">
+        <v>91.69</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -5348,6 +5809,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G154" t="n">
+        <v>39.92</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -5380,6 +5844,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G155" t="n">
+        <v>53.1</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -5412,6 +5879,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G156" t="n">
+        <v>26.88</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -5444,6 +5914,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G157" t="n">
+        <v>69.36</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -5476,6 +5949,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G158" t="n">
+        <v>80.81999999999999</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -5508,6 +5984,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G159" t="n">
+        <v>6.7</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -5540,6 +6019,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G160" t="n">
+        <v>81.48999999999999</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -5572,6 +6054,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G161" t="n">
+        <v>64.01000000000001</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -5604,6 +6089,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G162" t="n">
+        <v>67.73999999999999</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -5636,6 +6124,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G163" t="n">
+        <v>32.32</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -5668,6 +6159,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G164" t="n">
+        <v>26.56</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -5700,6 +6194,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G165" t="n">
+        <v>73.47</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -5732,6 +6229,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G166" t="n">
+        <v>42.59</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -5764,6 +6264,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G167" t="n">
+        <v>15.87</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -5796,6 +6299,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G168" t="n">
+        <v>99.38</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -5828,6 +6334,9 @@
           <t>OUT</t>
         </is>
       </c>
+      <c r="G169" t="n">
+        <v>13.88</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -5860,6 +6369,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G170" t="n">
+        <v>50.69</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -5892,6 +6404,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G171" t="n">
+        <v>9.92</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -5924,6 +6439,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G172" t="n">
+        <v>24.23</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -5956,6 +6474,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G173" t="n">
+        <v>39.9</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -5988,6 +6509,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G174" t="n">
+        <v>80.11</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -6020,6 +6544,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G175" t="n">
+        <v>34.2</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -6052,6 +6579,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G176" t="n">
+        <v>68.66</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -6084,6 +6614,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G177" t="n">
+        <v>15.43</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -6116,6 +6649,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G178" t="n">
+        <v>88.68000000000001</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -6148,6 +6684,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G179" t="n">
+        <v>58.2</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -6180,6 +6719,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G180" t="n">
+        <v>13.63</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -6212,6 +6754,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G181" t="n">
+        <v>5.43</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -6244,6 +6789,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G182" t="n">
+        <v>17.36</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -6276,6 +6824,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G183" t="n">
+        <v>71.55</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -6308,6 +6859,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G184" t="n">
+        <v>57.53</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -6340,6 +6894,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G185" t="n">
+        <v>53.11</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -6372,6 +6929,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G186" t="n">
+        <v>82.87</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -6404,6 +6964,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G187" t="n">
+        <v>49.32</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -6436,6 +6999,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G188" t="n">
+        <v>59.41</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -6468,6 +7034,9 @@
           <t>OUT</t>
         </is>
       </c>
+      <c r="G189" t="n">
+        <v>2.6</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -6500,6 +7069,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G190" t="n">
+        <v>9.130000000000001</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -6532,6 +7104,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G191" t="n">
+        <v>49.96</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -6564,6 +7139,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G192" t="n">
+        <v>3.52</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -6596,6 +7174,9 @@
           <t>OUT</t>
         </is>
       </c>
+      <c r="G193" t="n">
+        <v>11.35</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -6628,6 +7209,9 @@
           <t>QUESTIONABLE</t>
         </is>
       </c>
+      <c r="G194" t="n">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -6660,6 +7244,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G195" t="n">
+        <v>0.74</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -6692,6 +7279,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G196" t="n">
+        <v>40.34</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -6724,6 +7314,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G197" t="n">
+        <v>23.09</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -6756,6 +7349,9 @@
           <t>NORMAL</t>
         </is>
       </c>
+      <c r="G198" t="n">
+        <v>33.8</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -6788,6 +7384,9 @@
           <t>ACTIVE</t>
         </is>
       </c>
+      <c r="G199" t="n">
+        <v>3.54</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -6819,6 +7418,9 @@
         <is>
           <t>ACTIVE</t>
         </is>
+      </c>
+      <c r="G200" t="n">
+        <v>52.76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add LandingPage component with start flow
Introduces a new LandingPage component that displays the app title and a start button, shown after league data loads. Updates App to show the landing page before starting the comparison flow, and adjusts tests to cover the new flow. Adds styles and tests for the LandingPage component.
</commit_message>
<xml_diff>
--- a/data/roster_dub.xlsx
+++ b/data/roster_dub.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G200"/>
+  <dimension ref="A1:H200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,11 @@
           <t>Percent Started</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Pos Rank</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -490,7 +495,10 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>95.58</v>
+        <v>95.59</v>
+      </c>
+      <c r="H2" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -525,7 +533,10 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>95.89</v>
+        <v>95.86</v>
+      </c>
+      <c r="H3" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -562,6 +573,9 @@
       <c r="G4" t="n">
         <v>8.17</v>
       </c>
+      <c r="H4" t="n">
+        <v>41</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -595,7 +609,10 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>15.93</v>
+        <v>15.79</v>
+      </c>
+      <c r="H5" t="n">
+        <v>62</v>
       </c>
     </row>
     <row r="6">
@@ -630,7 +647,10 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>42.59</v>
+        <v>42.63</v>
+      </c>
+      <c r="H6" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="7">
@@ -665,7 +685,10 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>98.36</v>
+        <v>98.37</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -700,7 +723,10 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>6.43</v>
+        <v>6.38</v>
+      </c>
+      <c r="H8" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="9">
@@ -735,7 +761,10 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>38.23</v>
+        <v>38.24</v>
+      </c>
+      <c r="H9" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="10">
@@ -770,7 +799,10 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>74.62</v>
+        <v>75.33</v>
+      </c>
+      <c r="H10" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -805,7 +837,10 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>51.58</v>
+        <v>51.79</v>
+      </c>
+      <c r="H11" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="12">
@@ -840,7 +875,10 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>61.47</v>
+        <v>61.39</v>
+      </c>
+      <c r="H12" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="13">
@@ -875,7 +913,10 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>26.17</v>
+        <v>26.14</v>
+      </c>
+      <c r="H13" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="14">
@@ -910,7 +951,10 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>30.26</v>
+        <v>30.3</v>
+      </c>
+      <c r="H14" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -945,7 +989,10 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>1.22</v>
+        <v>1.25</v>
+      </c>
+      <c r="H15" t="n">
+        <v>62</v>
       </c>
     </row>
     <row r="16">
@@ -980,7 +1027,10 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>43.75</v>
+        <v>43.03</v>
+      </c>
+      <c r="H16" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="17">
@@ -1015,7 +1065,10 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>26.03</v>
+        <v>26.34</v>
+      </c>
+      <c r="H17" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="18">
@@ -1050,7 +1103,10 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>15.08</v>
+        <v>15.37</v>
+      </c>
+      <c r="H18" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="19">
@@ -1085,7 +1141,10 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>98.97</v>
+        <v>98.98</v>
+      </c>
+      <c r="H19" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -1120,7 +1179,10 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>42.75</v>
+        <v>43.02</v>
+      </c>
+      <c r="H20" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="21">
@@ -1155,7 +1217,10 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>47.36</v>
+        <v>46.44</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="22">
@@ -1190,7 +1255,10 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>75.58</v>
+        <v>75.75</v>
+      </c>
+      <c r="H22" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="23">
@@ -1225,7 +1293,10 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>23.08</v>
+        <v>23.4</v>
+      </c>
+      <c r="H23" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="24">
@@ -1260,7 +1331,10 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>46.18</v>
+        <v>46.13</v>
+      </c>
+      <c r="H24" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="25">
@@ -1295,7 +1369,10 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>34.89</v>
+        <v>34.95</v>
+      </c>
+      <c r="H25" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="26">
@@ -1330,7 +1407,10 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>21.61</v>
+        <v>21.75</v>
+      </c>
+      <c r="H26" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="27">
@@ -1365,7 +1445,10 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>27.72</v>
+        <v>26.97</v>
+      </c>
+      <c r="H27" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="28">
@@ -1402,6 +1485,9 @@
       <c r="G28" t="n">
         <v>2.02</v>
       </c>
+      <c r="H28" t="n">
+        <v>68</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1435,7 +1521,10 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>94.13</v>
+        <v>94.18000000000001</v>
+      </c>
+      <c r="H29" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="30">
@@ -1472,6 +1561,9 @@
       <c r="G30" t="n">
         <v>12.65</v>
       </c>
+      <c r="H30" t="n">
+        <v>52</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1505,7 +1597,10 @@
         </is>
       </c>
       <c r="G31" t="n">
-        <v>12.29</v>
+        <v>11.97</v>
+      </c>
+      <c r="H31" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="32">
@@ -1540,7 +1635,10 @@
         </is>
       </c>
       <c r="G32" t="n">
-        <v>62.69</v>
+        <v>62.86</v>
+      </c>
+      <c r="H32" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="33">
@@ -1575,7 +1673,10 @@
         </is>
       </c>
       <c r="G33" t="n">
-        <v>32.52</v>
+        <v>31.67</v>
+      </c>
+      <c r="H33" t="n">
+        <v>78</v>
       </c>
     </row>
     <row r="34">
@@ -1610,7 +1711,10 @@
         </is>
       </c>
       <c r="G34" t="n">
-        <v>26.68</v>
+        <v>27</v>
+      </c>
+      <c r="H34" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="35">
@@ -1645,7 +1749,10 @@
         </is>
       </c>
       <c r="G35" t="n">
-        <v>17.63</v>
+        <v>17.23</v>
+      </c>
+      <c r="H35" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="36">
@@ -1682,6 +1789,9 @@
       <c r="G36" t="n">
         <v>99.31999999999999</v>
       </c>
+      <c r="H36" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1715,7 +1825,10 @@
         </is>
       </c>
       <c r="G37" t="n">
-        <v>86.56</v>
+        <v>86.56999999999999</v>
+      </c>
+      <c r="H37" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="38">
@@ -1750,7 +1863,10 @@
         </is>
       </c>
       <c r="G38" t="n">
-        <v>37.6</v>
+        <v>36.92</v>
+      </c>
+      <c r="H38" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="39">
@@ -1785,7 +1901,10 @@
         </is>
       </c>
       <c r="G39" t="n">
-        <v>36.5</v>
+        <v>36.41</v>
+      </c>
+      <c r="H39" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="40">
@@ -1820,7 +1939,10 @@
         </is>
       </c>
       <c r="G40" t="n">
-        <v>84.01000000000001</v>
+        <v>84.02</v>
+      </c>
+      <c r="H40" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="41">
@@ -1855,7 +1977,10 @@
         </is>
       </c>
       <c r="G41" t="n">
-        <v>73.42</v>
+        <v>73.43000000000001</v>
+      </c>
+      <c r="H41" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="42">
@@ -1890,7 +2015,10 @@
         </is>
       </c>
       <c r="G42" t="n">
-        <v>41.17</v>
+        <v>41.67</v>
+      </c>
+      <c r="H42" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="43">
@@ -1925,7 +2053,10 @@
         </is>
       </c>
       <c r="G43" t="n">
-        <v>7.65</v>
+        <v>7.53</v>
+      </c>
+      <c r="H43" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="44">
@@ -1960,7 +2091,10 @@
         </is>
       </c>
       <c r="G44" t="n">
-        <v>9.369999999999999</v>
+        <v>9.23</v>
+      </c>
+      <c r="H44" t="n">
+        <v>102</v>
       </c>
     </row>
     <row r="45">
@@ -1997,6 +2131,9 @@
       <c r="G45" t="n">
         <v>24.87</v>
       </c>
+      <c r="H45" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2030,7 +2167,10 @@
         </is>
       </c>
       <c r="G46" t="n">
-        <v>36.12</v>
+        <v>35.93</v>
+      </c>
+      <c r="H46" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="47">
@@ -2065,7 +2205,10 @@
         </is>
       </c>
       <c r="G47" t="n">
-        <v>57.76</v>
+        <v>56.78</v>
+      </c>
+      <c r="H47" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="48">
@@ -2100,7 +2243,10 @@
         </is>
       </c>
       <c r="G48" t="n">
-        <v>18.18</v>
+        <v>18.46</v>
+      </c>
+      <c r="H48" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="49">
@@ -2135,7 +2281,10 @@
         </is>
       </c>
       <c r="G49" t="n">
-        <v>72.56</v>
+        <v>72.37</v>
+      </c>
+      <c r="H49" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="50">
@@ -2170,7 +2319,10 @@
         </is>
       </c>
       <c r="G50" t="n">
-        <v>24.1</v>
+        <v>24</v>
+      </c>
+      <c r="H50" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="51">
@@ -2205,7 +2357,10 @@
         </is>
       </c>
       <c r="G51" t="n">
-        <v>30.53</v>
+        <v>30.96</v>
+      </c>
+      <c r="H51" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="52">
@@ -2240,7 +2395,10 @@
         </is>
       </c>
       <c r="G52" t="n">
-        <v>12.2</v>
+        <v>12.19</v>
+      </c>
+      <c r="H52" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="53">
@@ -2275,7 +2433,10 @@
         </is>
       </c>
       <c r="G53" t="n">
-        <v>69.31</v>
+        <v>69.44</v>
+      </c>
+      <c r="H53" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="54">
@@ -2310,7 +2471,10 @@
         </is>
       </c>
       <c r="G54" t="n">
-        <v>56.63</v>
+        <v>56.32</v>
+      </c>
+      <c r="H54" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="55">
@@ -2347,6 +2511,9 @@
       <c r="G55" t="n">
         <v>0.28</v>
       </c>
+      <c r="H55" t="n">
+        <v>131</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2380,7 +2547,10 @@
         </is>
       </c>
       <c r="G56" t="n">
-        <v>74.03</v>
+        <v>74.06999999999999</v>
+      </c>
+      <c r="H56" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="57">
@@ -2415,7 +2585,10 @@
         </is>
       </c>
       <c r="G57" t="n">
-        <v>42.78</v>
+        <v>42.82</v>
+      </c>
+      <c r="H57" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="58">
@@ -2450,7 +2623,10 @@
         </is>
       </c>
       <c r="G58" t="n">
-        <v>26.06</v>
+        <v>25.42</v>
+      </c>
+      <c r="H58" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="59">
@@ -2485,7 +2661,10 @@
         </is>
       </c>
       <c r="G59" t="n">
-        <v>43.17</v>
+        <v>43.58</v>
+      </c>
+      <c r="H59" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="60">
@@ -2520,7 +2699,10 @@
         </is>
       </c>
       <c r="G60" t="n">
-        <v>43.01</v>
+        <v>43.48</v>
+      </c>
+      <c r="H60" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="61">
@@ -2555,7 +2737,10 @@
         </is>
       </c>
       <c r="G61" t="n">
-        <v>48.05</v>
+        <v>47.9</v>
+      </c>
+      <c r="H61" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="62">
@@ -2590,7 +2775,10 @@
         </is>
       </c>
       <c r="G62" t="n">
-        <v>78.38</v>
+        <v>78.45999999999999</v>
+      </c>
+      <c r="H62" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="63">
@@ -2625,7 +2813,10 @@
         </is>
       </c>
       <c r="G63" t="n">
-        <v>9.619999999999999</v>
+        <v>9.51</v>
+      </c>
+      <c r="H63" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="64">
@@ -2660,7 +2851,10 @@
         </is>
       </c>
       <c r="G64" t="n">
-        <v>3.67</v>
+        <v>3.68</v>
+      </c>
+      <c r="H64" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="65">
@@ -2695,7 +2889,10 @@
         </is>
       </c>
       <c r="G65" t="n">
-        <v>53.84</v>
+        <v>53.77</v>
+      </c>
+      <c r="H65" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="66">
@@ -2732,6 +2929,9 @@
       <c r="G66" t="n">
         <v>7.69</v>
       </c>
+      <c r="H66" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2765,7 +2965,10 @@
         </is>
       </c>
       <c r="G67" t="n">
-        <v>40.95</v>
+        <v>41.23</v>
+      </c>
+      <c r="H67" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="68">
@@ -2800,7 +3003,10 @@
         </is>
       </c>
       <c r="G68" t="n">
-        <v>4.43</v>
+        <v>4.57</v>
+      </c>
+      <c r="H68" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="69">
@@ -2835,7 +3041,10 @@
         </is>
       </c>
       <c r="G69" t="n">
-        <v>64.36</v>
+        <v>65.11</v>
+      </c>
+      <c r="H69" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="70">
@@ -2870,7 +3079,10 @@
         </is>
       </c>
       <c r="G70" t="n">
-        <v>16.43</v>
+        <v>16.62</v>
+      </c>
+      <c r="H70" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="71">
@@ -2905,7 +3117,10 @@
         </is>
       </c>
       <c r="G71" t="n">
-        <v>83.01000000000001</v>
+        <v>83.08</v>
+      </c>
+      <c r="H71" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="72">
@@ -2940,7 +3155,10 @@
         </is>
       </c>
       <c r="G72" t="n">
-        <v>52.64</v>
+        <v>53.07</v>
+      </c>
+      <c r="H72" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="73">
@@ -2975,7 +3193,10 @@
         </is>
       </c>
       <c r="G73" t="n">
-        <v>72.66</v>
+        <v>72.73</v>
+      </c>
+      <c r="H73" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="74">
@@ -3010,7 +3231,10 @@
         </is>
       </c>
       <c r="G74" t="n">
-        <v>72.13</v>
+        <v>72.26000000000001</v>
+      </c>
+      <c r="H74" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="75">
@@ -3045,7 +3269,10 @@
         </is>
       </c>
       <c r="G75" t="n">
-        <v>49.4</v>
+        <v>49.32</v>
+      </c>
+      <c r="H75" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="76">
@@ -3080,7 +3307,10 @@
         </is>
       </c>
       <c r="G76" t="n">
-        <v>28.32</v>
+        <v>27.61</v>
+      </c>
+      <c r="H76" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="77">
@@ -3115,7 +3345,10 @@
         </is>
       </c>
       <c r="G77" t="n">
-        <v>91.73</v>
+        <v>91.81999999999999</v>
+      </c>
+      <c r="H77" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="78">
@@ -3150,7 +3383,10 @@
         </is>
       </c>
       <c r="G78" t="n">
-        <v>37.19</v>
+        <v>37.02</v>
+      </c>
+      <c r="H78" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="79">
@@ -3185,7 +3421,10 @@
         </is>
       </c>
       <c r="G79" t="n">
-        <v>41.6</v>
+        <v>41.43</v>
+      </c>
+      <c r="H79" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="80">
@@ -3220,7 +3459,10 @@
         </is>
       </c>
       <c r="G80" t="n">
-        <v>70.70999999999999</v>
+        <v>70.63</v>
+      </c>
+      <c r="H80" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="81">
@@ -3255,7 +3497,10 @@
         </is>
       </c>
       <c r="G81" t="n">
-        <v>53.34</v>
+        <v>53.37</v>
+      </c>
+      <c r="H81" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="82">
@@ -3290,7 +3535,10 @@
         </is>
       </c>
       <c r="G82" t="n">
-        <v>52.43</v>
+        <v>52.81</v>
+      </c>
+      <c r="H82" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="83">
@@ -3325,7 +3573,10 @@
         </is>
       </c>
       <c r="G83" t="n">
-        <v>19.79</v>
+        <v>19.67</v>
+      </c>
+      <c r="H83" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="84">
@@ -3360,7 +3611,10 @@
         </is>
       </c>
       <c r="G84" t="n">
-        <v>4.64</v>
+        <v>4.7</v>
+      </c>
+      <c r="H84" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="85">
@@ -3395,7 +3649,10 @@
         </is>
       </c>
       <c r="G85" t="n">
-        <v>16.01</v>
+        <v>16.32</v>
+      </c>
+      <c r="H85" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="86">
@@ -3430,7 +3687,10 @@
         </is>
       </c>
       <c r="G86" t="n">
-        <v>71.98999999999999</v>
+        <v>72.75</v>
+      </c>
+      <c r="H86" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="87">
@@ -3465,7 +3725,10 @@
         </is>
       </c>
       <c r="G87" t="n">
-        <v>31.34</v>
+        <v>31.88</v>
+      </c>
+      <c r="H87" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="88">
@@ -3500,7 +3763,10 @@
         </is>
       </c>
       <c r="G88" t="n">
-        <v>89.47</v>
+        <v>89.45</v>
+      </c>
+      <c r="H88" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="89">
@@ -3537,6 +3803,9 @@
       <c r="G89" t="n">
         <v>0.84</v>
       </c>
+      <c r="H89" t="n">
+        <v>48</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3570,7 +3839,10 @@
         </is>
       </c>
       <c r="G90" t="n">
-        <v>22.09</v>
+        <v>21.54</v>
+      </c>
+      <c r="H90" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="91">
@@ -3607,6 +3879,9 @@
       <c r="G91" t="n">
         <v>0.08</v>
       </c>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3640,7 +3915,10 @@
         </is>
       </c>
       <c r="G92" t="n">
-        <v>24.59</v>
+        <v>24.17</v>
+      </c>
+      <c r="H92" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="93">
@@ -3675,7 +3953,10 @@
         </is>
       </c>
       <c r="G93" t="n">
-        <v>94.02</v>
+        <v>94.04000000000001</v>
+      </c>
+      <c r="H93" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="94">
@@ -3710,7 +3991,10 @@
         </is>
       </c>
       <c r="G94" t="n">
-        <v>8.02</v>
+        <v>7.94</v>
+      </c>
+      <c r="H94" t="n">
+        <v>71</v>
       </c>
     </row>
     <row r="95">
@@ -3745,7 +4029,10 @@
         </is>
       </c>
       <c r="G95" t="n">
-        <v>55.49</v>
+        <v>55.6</v>
+      </c>
+      <c r="H95" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="96">
@@ -3780,7 +4067,10 @@
         </is>
       </c>
       <c r="G96" t="n">
-        <v>17.87</v>
+        <v>18.02</v>
+      </c>
+      <c r="H96" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="97">
@@ -3815,7 +4105,10 @@
         </is>
       </c>
       <c r="G97" t="n">
-        <v>27.8</v>
+        <v>27.59</v>
+      </c>
+      <c r="H97" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="98">
@@ -3850,7 +4143,10 @@
         </is>
       </c>
       <c r="G98" t="n">
-        <v>5.19</v>
+        <v>5.01</v>
+      </c>
+      <c r="H98" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="99">
@@ -3885,7 +4181,10 @@
         </is>
       </c>
       <c r="G99" t="n">
-        <v>63.11</v>
+        <v>63.9</v>
+      </c>
+      <c r="H99" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="100">
@@ -3920,7 +4219,10 @@
         </is>
       </c>
       <c r="G100" t="n">
-        <v>1.08</v>
+        <v>1.07</v>
+      </c>
+      <c r="H100" t="n">
+        <v>76</v>
       </c>
     </row>
     <row r="101">
@@ -3957,6 +4259,9 @@
       <c r="G101" t="n">
         <v>1.26</v>
       </c>
+      <c r="H101" t="n">
+        <v>58</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3990,7 +4295,10 @@
         </is>
       </c>
       <c r="G102" t="n">
-        <v>17.19</v>
+        <v>17.1</v>
+      </c>
+      <c r="H102" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="103">
@@ -4025,7 +4333,10 @@
         </is>
       </c>
       <c r="G103" t="n">
-        <v>44.51</v>
+        <v>45.41</v>
+      </c>
+      <c r="H103" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="104">
@@ -4060,7 +4371,10 @@
         </is>
       </c>
       <c r="G104" t="n">
-        <v>72.34999999999999</v>
+        <v>73.06999999999999</v>
+      </c>
+      <c r="H104" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="105">
@@ -4095,7 +4409,10 @@
         </is>
       </c>
       <c r="G105" t="n">
-        <v>55.95</v>
+        <v>55.85</v>
+      </c>
+      <c r="H105" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="106">
@@ -4130,7 +4447,10 @@
         </is>
       </c>
       <c r="G106" t="n">
-        <v>4.91</v>
+        <v>4.86</v>
+      </c>
+      <c r="H106" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="107">
@@ -4165,7 +4485,10 @@
         </is>
       </c>
       <c r="G107" t="n">
-        <v>14.81</v>
+        <v>14.95</v>
+      </c>
+      <c r="H107" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="108">
@@ -4200,7 +4523,10 @@
         </is>
       </c>
       <c r="G108" t="n">
-        <v>73.41</v>
+        <v>73.59</v>
+      </c>
+      <c r="H108" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="109">
@@ -4235,7 +4561,10 @@
         </is>
       </c>
       <c r="G109" t="n">
-        <v>16.88</v>
+        <v>16.85</v>
+      </c>
+      <c r="H109" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="110">
@@ -4270,7 +4599,10 @@
         </is>
       </c>
       <c r="G110" t="n">
-        <v>7.43</v>
+        <v>7.42</v>
+      </c>
+      <c r="H110" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="111">
@@ -4305,7 +4637,10 @@
         </is>
       </c>
       <c r="G111" t="n">
-        <v>64.79000000000001</v>
+        <v>64.45999999999999</v>
+      </c>
+      <c r="H111" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="112">
@@ -4340,7 +4675,10 @@
         </is>
       </c>
       <c r="G112" t="n">
-        <v>18.9</v>
+        <v>18.78</v>
+      </c>
+      <c r="H112" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="113">
@@ -4375,7 +4713,10 @@
         </is>
       </c>
       <c r="G113" t="n">
-        <v>46.18</v>
+        <v>45.31</v>
+      </c>
+      <c r="H113" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="114">
@@ -4410,7 +4751,10 @@
         </is>
       </c>
       <c r="G114" t="n">
-        <v>29.68</v>
+        <v>29.77</v>
+      </c>
+      <c r="H114" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="115">
@@ -4445,7 +4789,10 @@
         </is>
       </c>
       <c r="G115" t="n">
-        <v>12.77</v>
+        <v>12.42</v>
+      </c>
+      <c r="H115" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="116">
@@ -4480,7 +4827,10 @@
         </is>
       </c>
       <c r="G116" t="n">
-        <v>66.97</v>
+        <v>66.70999999999999</v>
+      </c>
+      <c r="H116" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="117">
@@ -4515,7 +4865,10 @@
         </is>
       </c>
       <c r="G117" t="n">
-        <v>14.56</v>
+        <v>14.63</v>
+      </c>
+      <c r="H117" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="118">
@@ -4550,7 +4903,10 @@
         </is>
       </c>
       <c r="G118" t="n">
-        <v>37.99</v>
+        <v>37.79</v>
+      </c>
+      <c r="H118" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="119">
@@ -4585,7 +4941,10 @@
         </is>
       </c>
       <c r="G119" t="n">
-        <v>75.62</v>
+        <v>75.73</v>
+      </c>
+      <c r="H119" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="120">
@@ -4620,7 +4979,10 @@
         </is>
       </c>
       <c r="G120" t="n">
-        <v>94.44</v>
+        <v>94.42</v>
+      </c>
+      <c r="H120" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -4655,7 +5017,10 @@
         </is>
       </c>
       <c r="G121" t="n">
-        <v>79.42</v>
+        <v>79.40000000000001</v>
+      </c>
+      <c r="H121" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="122">
@@ -4690,7 +5055,10 @@
         </is>
       </c>
       <c r="G122" t="n">
-        <v>24.1</v>
+        <v>23.86</v>
+      </c>
+      <c r="H122" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="123">
@@ -4725,7 +5093,10 @@
         </is>
       </c>
       <c r="G123" t="n">
-        <v>28.52</v>
+        <v>27.78</v>
+      </c>
+      <c r="H123" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="124">
@@ -4760,7 +5131,10 @@
         </is>
       </c>
       <c r="G124" t="n">
-        <v>14.37</v>
+        <v>14.12</v>
+      </c>
+      <c r="H124" t="n">
+        <v>66</v>
       </c>
     </row>
     <row r="125">
@@ -4795,7 +5169,10 @@
         </is>
       </c>
       <c r="G125" t="n">
-        <v>65.84</v>
+        <v>66.48999999999999</v>
+      </c>
+      <c r="H125" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="126">
@@ -4830,7 +5207,10 @@
         </is>
       </c>
       <c r="G126" t="n">
-        <v>58.82</v>
+        <v>58.66</v>
+      </c>
+      <c r="H126" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="127">
@@ -4865,7 +5245,10 @@
         </is>
       </c>
       <c r="G127" t="n">
-        <v>46.37</v>
+        <v>46.18</v>
+      </c>
+      <c r="H127" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="128">
@@ -4900,7 +5283,10 @@
         </is>
       </c>
       <c r="G128" t="n">
-        <v>68.52</v>
+        <v>69.20999999999999</v>
+      </c>
+      <c r="H128" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="129">
@@ -4935,7 +5321,10 @@
         </is>
       </c>
       <c r="G129" t="n">
-        <v>10.76</v>
+        <v>10.94</v>
+      </c>
+      <c r="H129" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="130">
@@ -4970,7 +5359,10 @@
         </is>
       </c>
       <c r="G130" t="n">
-        <v>13.5</v>
+        <v>13.7</v>
+      </c>
+      <c r="H130" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="131">
@@ -5005,7 +5397,10 @@
         </is>
       </c>
       <c r="G131" t="n">
-        <v>7.51</v>
+        <v>7.38</v>
+      </c>
+      <c r="H131" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="132">
@@ -5040,7 +5435,10 @@
         </is>
       </c>
       <c r="G132" t="n">
-        <v>20.73</v>
+        <v>20.71</v>
+      </c>
+      <c r="H132" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="133">
@@ -5075,7 +5473,10 @@
         </is>
       </c>
       <c r="G133" t="n">
-        <v>6.97</v>
+        <v>6.99</v>
+      </c>
+      <c r="H133" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="134">
@@ -5110,7 +5511,10 @@
         </is>
       </c>
       <c r="G134" t="n">
-        <v>30.39</v>
+        <v>29.69</v>
+      </c>
+      <c r="H134" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="135">
@@ -5145,7 +5549,10 @@
         </is>
       </c>
       <c r="G135" t="n">
-        <v>73.87</v>
+        <v>74.52</v>
+      </c>
+      <c r="H135" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="136">
@@ -5180,7 +5587,10 @@
         </is>
       </c>
       <c r="G136" t="n">
-        <v>61.65</v>
+        <v>62.42</v>
+      </c>
+      <c r="H136" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="137">
@@ -5217,6 +5627,9 @@
       <c r="G137" t="n">
         <v>4.21</v>
       </c>
+      <c r="H137" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -5250,7 +5663,10 @@
         </is>
       </c>
       <c r="G138" t="n">
-        <v>82.40000000000001</v>
+        <v>82.43000000000001</v>
+      </c>
+      <c r="H138" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="139">
@@ -5285,7 +5701,10 @@
         </is>
       </c>
       <c r="G139" t="n">
-        <v>17.35</v>
+        <v>17.25</v>
+      </c>
+      <c r="H139" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="140">
@@ -5322,6 +5741,9 @@
       <c r="G140" t="n">
         <v>0.51</v>
       </c>
+      <c r="H140" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -5355,7 +5777,10 @@
         </is>
       </c>
       <c r="G141" t="n">
-        <v>84.72</v>
+        <v>84.73999999999999</v>
+      </c>
+      <c r="H141" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="142">
@@ -5392,6 +5817,9 @@
       <c r="G142" t="n">
         <v>0.6899999999999999</v>
       </c>
+      <c r="H142" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -5425,7 +5853,10 @@
         </is>
       </c>
       <c r="G143" t="n">
-        <v>70.01000000000001</v>
+        <v>69.84999999999999</v>
+      </c>
+      <c r="H143" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -5462,6 +5893,9 @@
       <c r="G144" t="n">
         <v>98.19</v>
       </c>
+      <c r="H144" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -5495,7 +5929,10 @@
         </is>
       </c>
       <c r="G145" t="n">
-        <v>86.02</v>
+        <v>86.04000000000001</v>
+      </c>
+      <c r="H145" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="146">
@@ -5532,6 +5969,9 @@
       <c r="G146" t="n">
         <v>1.31</v>
       </c>
+      <c r="H146" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -5565,7 +6005,10 @@
         </is>
       </c>
       <c r="G147" t="n">
-        <v>71.08</v>
+        <v>71.45</v>
+      </c>
+      <c r="H147" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="148">
@@ -5600,7 +6043,10 @@
         </is>
       </c>
       <c r="G148" t="n">
-        <v>1.71</v>
+        <v>1.66</v>
+      </c>
+      <c r="H148" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="149">
@@ -5635,7 +6081,10 @@
         </is>
       </c>
       <c r="G149" t="n">
-        <v>24.59</v>
+        <v>25.16</v>
+      </c>
+      <c r="H149" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="150">
@@ -5670,7 +6119,10 @@
         </is>
       </c>
       <c r="G150" t="n">
-        <v>0.86</v>
+        <v>0.85</v>
+      </c>
+      <c r="H150" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="151">
@@ -5705,7 +6157,10 @@
         </is>
       </c>
       <c r="G151" t="n">
-        <v>18.15</v>
+        <v>18.46</v>
+      </c>
+      <c r="H151" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="152">
@@ -5742,6 +6197,9 @@
       <c r="G152" t="n">
         <v>99.59</v>
       </c>
+      <c r="H152" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -5775,7 +6233,10 @@
         </is>
       </c>
       <c r="G153" t="n">
-        <v>91.69</v>
+        <v>91.76000000000001</v>
+      </c>
+      <c r="H153" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="154">
@@ -5810,7 +6271,10 @@
         </is>
       </c>
       <c r="G154" t="n">
-        <v>39.92</v>
+        <v>39.22</v>
+      </c>
+      <c r="H154" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="155">
@@ -5845,7 +6309,10 @@
         </is>
       </c>
       <c r="G155" t="n">
-        <v>53.1</v>
+        <v>53.65</v>
+      </c>
+      <c r="H155" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="156">
@@ -5880,7 +6347,10 @@
         </is>
       </c>
       <c r="G156" t="n">
-        <v>26.88</v>
+        <v>26.58</v>
+      </c>
+      <c r="H156" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="157">
@@ -5915,7 +6385,10 @@
         </is>
       </c>
       <c r="G157" t="n">
-        <v>69.36</v>
+        <v>69.48</v>
+      </c>
+      <c r="H157" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="158">
@@ -5950,7 +6423,10 @@
         </is>
       </c>
       <c r="G158" t="n">
-        <v>80.81999999999999</v>
+        <v>80.64</v>
+      </c>
+      <c r="H158" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="159">
@@ -5985,7 +6461,10 @@
         </is>
       </c>
       <c r="G159" t="n">
-        <v>6.7</v>
+        <v>6.6</v>
+      </c>
+      <c r="H159" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="160">
@@ -6020,7 +6499,10 @@
         </is>
       </c>
       <c r="G160" t="n">
-        <v>81.48999999999999</v>
+        <v>81.48</v>
+      </c>
+      <c r="H160" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="161">
@@ -6055,7 +6537,10 @@
         </is>
       </c>
       <c r="G161" t="n">
-        <v>64.01000000000001</v>
+        <v>64.67</v>
+      </c>
+      <c r="H161" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="162">
@@ -6090,7 +6575,10 @@
         </is>
       </c>
       <c r="G162" t="n">
-        <v>67.73999999999999</v>
+        <v>67.56999999999999</v>
+      </c>
+      <c r="H162" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="163">
@@ -6125,7 +6613,10 @@
         </is>
       </c>
       <c r="G163" t="n">
-        <v>32.32</v>
+        <v>32.09</v>
+      </c>
+      <c r="H163" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="164">
@@ -6160,7 +6651,10 @@
         </is>
       </c>
       <c r="G164" t="n">
-        <v>26.56</v>
+        <v>26.05</v>
+      </c>
+      <c r="H164" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="165">
@@ -6195,7 +6689,10 @@
         </is>
       </c>
       <c r="G165" t="n">
-        <v>73.47</v>
+        <v>73.43000000000001</v>
+      </c>
+      <c r="H165" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="166">
@@ -6230,7 +6727,10 @@
         </is>
       </c>
       <c r="G166" t="n">
-        <v>42.59</v>
+        <v>43.11</v>
+      </c>
+      <c r="H166" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="167">
@@ -6267,6 +6767,9 @@
       <c r="G167" t="n">
         <v>15.87</v>
       </c>
+      <c r="H167" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -6302,6 +6805,9 @@
       <c r="G168" t="n">
         <v>99.38</v>
       </c>
+      <c r="H168" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -6335,7 +6841,10 @@
         </is>
       </c>
       <c r="G169" t="n">
-        <v>13.88</v>
+        <v>13.85</v>
+      </c>
+      <c r="H169" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="170">
@@ -6370,7 +6879,10 @@
         </is>
       </c>
       <c r="G170" t="n">
-        <v>50.69</v>
+        <v>50.64</v>
+      </c>
+      <c r="H170" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="171">
@@ -6405,7 +6917,10 @@
         </is>
       </c>
       <c r="G171" t="n">
-        <v>9.92</v>
+        <v>10.18</v>
+      </c>
+      <c r="H171" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="172">
@@ -6440,7 +6955,10 @@
         </is>
       </c>
       <c r="G172" t="n">
-        <v>24.23</v>
+        <v>24.48</v>
+      </c>
+      <c r="H172" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="173">
@@ -6475,7 +6993,10 @@
         </is>
       </c>
       <c r="G173" t="n">
-        <v>39.9</v>
+        <v>39.83</v>
+      </c>
+      <c r="H173" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="174">
@@ -6510,7 +7031,10 @@
         </is>
       </c>
       <c r="G174" t="n">
-        <v>80.11</v>
+        <v>80.23</v>
+      </c>
+      <c r="H174" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="175">
@@ -6545,7 +7069,10 @@
         </is>
       </c>
       <c r="G175" t="n">
-        <v>34.2</v>
+        <v>34.08</v>
+      </c>
+      <c r="H175" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="176">
@@ -6580,7 +7107,10 @@
         </is>
       </c>
       <c r="G176" t="n">
-        <v>68.66</v>
+        <v>68.55</v>
+      </c>
+      <c r="H176" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="177">
@@ -6615,7 +7145,10 @@
         </is>
       </c>
       <c r="G177" t="n">
-        <v>15.43</v>
+        <v>15.34</v>
+      </c>
+      <c r="H177" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="178">
@@ -6650,7 +7183,10 @@
         </is>
       </c>
       <c r="G178" t="n">
-        <v>88.68000000000001</v>
+        <v>88.59999999999999</v>
+      </c>
+      <c r="H178" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="179">
@@ -6685,7 +7221,10 @@
         </is>
       </c>
       <c r="G179" t="n">
-        <v>58.2</v>
+        <v>58.05</v>
+      </c>
+      <c r="H179" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="180">
@@ -6720,7 +7259,10 @@
         </is>
       </c>
       <c r="G180" t="n">
-        <v>13.63</v>
+        <v>13.62</v>
+      </c>
+      <c r="H180" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="181">
@@ -6755,7 +7297,10 @@
         </is>
       </c>
       <c r="G181" t="n">
-        <v>5.43</v>
+        <v>5.36</v>
+      </c>
+      <c r="H181" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="182">
@@ -6790,7 +7335,10 @@
         </is>
       </c>
       <c r="G182" t="n">
-        <v>17.36</v>
+        <v>17.14</v>
+      </c>
+      <c r="H182" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="183">
@@ -6825,7 +7373,10 @@
         </is>
       </c>
       <c r="G183" t="n">
-        <v>71.55</v>
+        <v>71.67</v>
+      </c>
+      <c r="H183" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="184">
@@ -6860,7 +7411,10 @@
         </is>
       </c>
       <c r="G184" t="n">
-        <v>57.53</v>
+        <v>58.2</v>
+      </c>
+      <c r="H184" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="185">
@@ -6895,7 +7449,10 @@
         </is>
       </c>
       <c r="G185" t="n">
-        <v>53.11</v>
+        <v>53.55</v>
+      </c>
+      <c r="H185" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="186">
@@ -6930,7 +7487,10 @@
         </is>
       </c>
       <c r="G186" t="n">
-        <v>82.87</v>
+        <v>82.84</v>
+      </c>
+      <c r="H186" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="187">
@@ -6965,7 +7525,10 @@
         </is>
       </c>
       <c r="G187" t="n">
-        <v>49.32</v>
+        <v>49.13</v>
+      </c>
+      <c r="H187" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="188">
@@ -7000,7 +7563,10 @@
         </is>
       </c>
       <c r="G188" t="n">
-        <v>59.41</v>
+        <v>59.48</v>
+      </c>
+      <c r="H188" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="189">
@@ -7037,6 +7603,9 @@
       <c r="G189" t="n">
         <v>2.6</v>
       </c>
+      <c r="H189" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -7070,7 +7639,10 @@
         </is>
       </c>
       <c r="G190" t="n">
-        <v>9.130000000000001</v>
+        <v>8.949999999999999</v>
+      </c>
+      <c r="H190" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="191">
@@ -7105,7 +7677,10 @@
         </is>
       </c>
       <c r="G191" t="n">
-        <v>49.96</v>
+        <v>49.72</v>
+      </c>
+      <c r="H191" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="192">
@@ -7140,7 +7715,10 @@
         </is>
       </c>
       <c r="G192" t="n">
-        <v>3.52</v>
+        <v>3.44</v>
+      </c>
+      <c r="H192" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="193">
@@ -7175,7 +7753,10 @@
         </is>
       </c>
       <c r="G193" t="n">
-        <v>11.35</v>
+        <v>11.34</v>
+      </c>
+      <c r="H193" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="194">
@@ -7210,7 +7791,10 @@
         </is>
       </c>
       <c r="G194" t="n">
-        <v>4.5</v>
+        <v>4.52</v>
+      </c>
+      <c r="H194" t="n">
+        <v>132</v>
       </c>
     </row>
     <row r="195">
@@ -7245,7 +7829,10 @@
         </is>
       </c>
       <c r="G195" t="n">
-        <v>0.74</v>
+        <v>0.73</v>
+      </c>
+      <c r="H195" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="196">
@@ -7280,7 +7867,10 @@
         </is>
       </c>
       <c r="G196" t="n">
-        <v>40.34</v>
+        <v>40.99</v>
+      </c>
+      <c r="H196" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="197">
@@ -7315,7 +7905,10 @@
         </is>
       </c>
       <c r="G197" t="n">
-        <v>23.09</v>
+        <v>22.99</v>
+      </c>
+      <c r="H197" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="198">
@@ -7350,7 +7943,10 @@
         </is>
       </c>
       <c r="G198" t="n">
-        <v>33.8</v>
+        <v>34.57</v>
+      </c>
+      <c r="H198" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="199">
@@ -7385,7 +7981,10 @@
         </is>
       </c>
       <c r="G199" t="n">
-        <v>3.54</v>
+        <v>3.62</v>
+      </c>
+      <c r="H199" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="200">
@@ -7420,7 +8019,10 @@
         </is>
       </c>
       <c r="G200" t="n">
-        <v>52.76</v>
+        <v>53.4</v>
+      </c>
+      <c r="H200" t="n">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add owner name support and restart flow to rankings
This update adds support for displaying team owner names throughout the ranking flow, including parsing owner names from the Excel file and updating the Team and related components. A 'Rank Again' button is added to the RankingsScreen to allow users to restart the ranking process. Visual enhancements for top 3 teams and improved test coverage for these features are also included.
</commit_message>
<xml_diff>
--- a/data/roster_dub.xlsx
+++ b/data/roster_dub.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H200"/>
+  <dimension ref="A1:I200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,7 +459,12 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Pos Rank</t>
+          <t>Pos</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Owner Name</t>
         </is>
       </c>
     </row>
@@ -495,11 +500,16 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>95.59</v>
+        <v>95.61</v>
       </c>
       <c r="H2" t="n">
         <v>16</v>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -533,11 +543,16 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>95.86</v>
+        <v>95.83</v>
       </c>
       <c r="H3" t="n">
         <v>8</v>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -576,6 +591,11 @@
       <c r="H4" t="n">
         <v>41</v>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -609,11 +629,16 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>15.79</v>
+        <v>15.66</v>
       </c>
       <c r="H5" t="n">
         <v>62</v>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -647,11 +672,16 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>42.63</v>
+        <v>42.67</v>
       </c>
       <c r="H6" t="n">
         <v>21</v>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -685,11 +715,16 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>98.37</v>
+        <v>98.38</v>
       </c>
       <c r="H7" t="n">
         <v>1</v>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -723,11 +758,16 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>6.38</v>
+        <v>6.33</v>
       </c>
       <c r="H8" t="n">
         <v>46</v>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -761,11 +801,16 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>38.24</v>
+        <v>38.25</v>
       </c>
       <c r="H9" t="n">
         <v>11</v>
       </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -799,11 +844,16 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>75.33</v>
+        <v>75.98999999999999</v>
       </c>
       <c r="H10" t="n">
         <v>6</v>
       </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -837,11 +887,16 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>51.79</v>
+        <v>51.98</v>
       </c>
       <c r="H11" t="n">
         <v>21</v>
       </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -875,11 +930,16 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>61.39</v>
+        <v>61.3</v>
       </c>
       <c r="H12" t="n">
         <v>18</v>
       </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -913,11 +973,16 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>26.14</v>
+        <v>26.11</v>
       </c>
       <c r="H13" t="n">
         <v>42</v>
       </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -951,11 +1016,16 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>30.3</v>
+        <v>30.33</v>
       </c>
       <c r="H14" t="n">
         <v>10</v>
       </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -989,11 +1059,16 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>1.25</v>
+        <v>1.28</v>
       </c>
       <c r="H15" t="n">
         <v>62</v>
       </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1027,11 +1102,16 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>43.03</v>
+        <v>42.36</v>
       </c>
       <c r="H16" t="n">
         <v>11</v>
       </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1065,11 +1145,16 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>26.34</v>
+        <v>26.62</v>
       </c>
       <c r="H17" t="n">
         <v>31</v>
       </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1103,11 +1188,16 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>15.37</v>
+        <v>15.64</v>
       </c>
       <c r="H18" t="n">
         <v>18</v>
       </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Matt McIsaac</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1146,6 +1236,11 @@
       <c r="H19" t="n">
         <v>3</v>
       </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1179,11 +1274,16 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>43.02</v>
+        <v>43.28</v>
       </c>
       <c r="H20" t="n">
         <v>35</v>
       </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1217,11 +1317,16 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>46.44</v>
+        <v>45.58</v>
       </c>
       <c r="H21" t="n">
         <v>2</v>
       </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1255,11 +1360,16 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>75.75</v>
+        <v>75.92</v>
       </c>
       <c r="H22" t="n">
         <v>41</v>
       </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1293,11 +1403,16 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>23.4</v>
+        <v>23.71</v>
       </c>
       <c r="H23" t="n">
         <v>43</v>
       </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1331,11 +1446,16 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>46.13</v>
+        <v>46.09</v>
       </c>
       <c r="H24" t="n">
         <v>42</v>
       </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1369,11 +1489,16 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>34.95</v>
+        <v>35</v>
       </c>
       <c r="H25" t="n">
         <v>33</v>
       </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1407,11 +1532,16 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>21.75</v>
+        <v>21.88</v>
       </c>
       <c r="H26" t="n">
         <v>67</v>
       </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1445,11 +1575,16 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>26.97</v>
+        <v>26.28</v>
       </c>
       <c r="H27" t="n">
         <v>21</v>
       </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1483,11 +1618,16 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>2.02</v>
+        <v>2.01</v>
       </c>
       <c r="H28" t="n">
         <v>68</v>
       </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1521,11 +1661,16 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>94.18000000000001</v>
+        <v>94.23</v>
       </c>
       <c r="H29" t="n">
         <v>4</v>
       </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1564,6 +1709,11 @@
       <c r="H30" t="n">
         <v>52</v>
       </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1597,11 +1747,16 @@
         </is>
       </c>
       <c r="G31" t="n">
-        <v>11.97</v>
+        <v>11.68</v>
       </c>
       <c r="H31" t="n">
         <v>7</v>
       </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1635,11 +1790,16 @@
         </is>
       </c>
       <c r="G32" t="n">
-        <v>62.86</v>
+        <v>63.02</v>
       </c>
       <c r="H32" t="n">
         <v>20</v>
       </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1673,11 +1833,16 @@
         </is>
       </c>
       <c r="G33" t="n">
-        <v>31.67</v>
+        <v>30.92</v>
       </c>
       <c r="H33" t="n">
         <v>78</v>
       </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1711,11 +1876,16 @@
         </is>
       </c>
       <c r="G34" t="n">
-        <v>27</v>
+        <v>27.3</v>
       </c>
       <c r="H34" t="n">
         <v>10</v>
       </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1749,11 +1919,16 @@
         </is>
       </c>
       <c r="G35" t="n">
-        <v>17.23</v>
+        <v>16.86</v>
       </c>
       <c r="H35" t="n">
         <v>4</v>
       </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Leon Ruiter</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1792,6 +1967,11 @@
       <c r="H36" t="n">
         <v>1</v>
       </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1825,11 +2005,16 @@
         </is>
       </c>
       <c r="G37" t="n">
-        <v>86.56999999999999</v>
+        <v>86.58</v>
       </c>
       <c r="H37" t="n">
         <v>7</v>
       </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1863,11 +2048,16 @@
         </is>
       </c>
       <c r="G38" t="n">
-        <v>36.92</v>
+        <v>36.3</v>
       </c>
       <c r="H38" t="n">
         <v>12</v>
       </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1901,11 +2091,16 @@
         </is>
       </c>
       <c r="G39" t="n">
-        <v>36.41</v>
+        <v>36.31</v>
       </c>
       <c r="H39" t="n">
         <v>40</v>
       </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1939,11 +2134,16 @@
         </is>
       </c>
       <c r="G40" t="n">
-        <v>84.02</v>
+        <v>84.03</v>
       </c>
       <c r="H40" t="n">
         <v>5</v>
       </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1982,6 +2182,11 @@
       <c r="H41" t="n">
         <v>24</v>
       </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2015,11 +2220,16 @@
         </is>
       </c>
       <c r="G42" t="n">
-        <v>41.67</v>
+        <v>42.13</v>
       </c>
       <c r="H42" t="n">
         <v>20</v>
       </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2053,11 +2263,16 @@
         </is>
       </c>
       <c r="G43" t="n">
-        <v>7.53</v>
+        <v>7.43</v>
       </c>
       <c r="H43" t="n">
         <v>16</v>
       </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2091,11 +2306,16 @@
         </is>
       </c>
       <c r="G44" t="n">
-        <v>9.23</v>
+        <v>9.09</v>
       </c>
       <c r="H44" t="n">
         <v>102</v>
       </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2134,6 +2354,11 @@
       <c r="H45" t="n">
         <v>15</v>
       </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2167,11 +2392,16 @@
         </is>
       </c>
       <c r="G46" t="n">
-        <v>35.93</v>
+        <v>35.75</v>
       </c>
       <c r="H46" t="n">
         <v>13</v>
       </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2205,11 +2435,16 @@
         </is>
       </c>
       <c r="G47" t="n">
-        <v>56.78</v>
+        <v>55.89</v>
       </c>
       <c r="H47" t="n">
         <v>2</v>
       </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2243,11 +2478,16 @@
         </is>
       </c>
       <c r="G48" t="n">
-        <v>18.46</v>
+        <v>18.73</v>
       </c>
       <c r="H48" t="n">
         <v>38</v>
       </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2281,11 +2521,16 @@
         </is>
       </c>
       <c r="G49" t="n">
-        <v>72.37</v>
+        <v>72.19</v>
       </c>
       <c r="H49" t="n">
         <v>14</v>
       </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2319,11 +2564,16 @@
         </is>
       </c>
       <c r="G50" t="n">
-        <v>24</v>
+        <v>23.9</v>
       </c>
       <c r="H50" t="n">
         <v>15</v>
       </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2357,11 +2607,16 @@
         </is>
       </c>
       <c r="G51" t="n">
-        <v>30.96</v>
+        <v>31.35</v>
       </c>
       <c r="H51" t="n">
         <v>26</v>
       </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Matthew Haid</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2395,11 +2650,16 @@
         </is>
       </c>
       <c r="G52" t="n">
-        <v>12.19</v>
+        <v>12.18</v>
       </c>
       <c r="H52" t="n">
         <v>27</v>
       </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2433,11 +2693,16 @@
         </is>
       </c>
       <c r="G53" t="n">
-        <v>69.44</v>
+        <v>69.56</v>
       </c>
       <c r="H53" t="n">
         <v>13</v>
       </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2471,11 +2736,16 @@
         </is>
       </c>
       <c r="G54" t="n">
-        <v>56.32</v>
+        <v>56.03</v>
       </c>
       <c r="H54" t="n">
         <v>5</v>
       </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2514,6 +2784,11 @@
       <c r="H55" t="n">
         <v>131</v>
       </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2547,11 +2822,16 @@
         </is>
       </c>
       <c r="G56" t="n">
-        <v>74.06999999999999</v>
+        <v>74.11</v>
       </c>
       <c r="H56" t="n">
         <v>2</v>
       </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2585,11 +2865,16 @@
         </is>
       </c>
       <c r="G57" t="n">
-        <v>42.82</v>
+        <v>42.87</v>
       </c>
       <c r="H57" t="n">
         <v>19</v>
       </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2623,11 +2908,16 @@
         </is>
       </c>
       <c r="G58" t="n">
-        <v>25.42</v>
+        <v>24.82</v>
       </c>
       <c r="H58" t="n">
         <v>7</v>
       </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2661,11 +2951,16 @@
         </is>
       </c>
       <c r="G59" t="n">
-        <v>43.58</v>
+        <v>43.95</v>
       </c>
       <c r="H59" t="n">
         <v>28</v>
       </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2699,11 +2994,16 @@
         </is>
       </c>
       <c r="G60" t="n">
-        <v>43.48</v>
+        <v>43.92</v>
       </c>
       <c r="H60" t="n">
         <v>37</v>
       </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2737,11 +3037,16 @@
         </is>
       </c>
       <c r="G61" t="n">
-        <v>47.9</v>
+        <v>47.76</v>
       </c>
       <c r="H61" t="n">
         <v>29</v>
       </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2775,11 +3080,16 @@
         </is>
       </c>
       <c r="G62" t="n">
-        <v>78.45999999999999</v>
+        <v>78.53</v>
       </c>
       <c r="H62" t="n">
         <v>18</v>
       </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2813,11 +3123,16 @@
         </is>
       </c>
       <c r="G63" t="n">
-        <v>9.51</v>
+        <v>9.42</v>
       </c>
       <c r="H63" t="n">
         <v>49</v>
       </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2856,6 +3171,11 @@
       <c r="H64" t="n">
         <v>55</v>
       </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2889,11 +3209,16 @@
         </is>
       </c>
       <c r="G65" t="n">
-        <v>53.77</v>
+        <v>53.7</v>
       </c>
       <c r="H65" t="n">
         <v>2</v>
       </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2932,6 +3257,11 @@
       <c r="H66" t="n">
         <v>50</v>
       </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2965,11 +3295,16 @@
         </is>
       </c>
       <c r="G67" t="n">
-        <v>41.23</v>
+        <v>41.5</v>
       </c>
       <c r="H67" t="n">
         <v>14</v>
       </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3003,11 +3338,16 @@
         </is>
       </c>
       <c r="G68" t="n">
-        <v>4.57</v>
+        <v>4.72</v>
       </c>
       <c r="H68" t="n">
         <v>69</v>
       </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>Timothy Kubik</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3041,11 +3381,16 @@
         </is>
       </c>
       <c r="G69" t="n">
-        <v>65.11</v>
+        <v>65.78</v>
       </c>
       <c r="H69" t="n">
         <v>12</v>
       </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3079,11 +3424,16 @@
         </is>
       </c>
       <c r="G70" t="n">
-        <v>16.62</v>
+        <v>16.79</v>
       </c>
       <c r="H70" t="n">
         <v>51</v>
       </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3117,11 +3467,16 @@
         </is>
       </c>
       <c r="G71" t="n">
-        <v>83.08</v>
+        <v>83.14</v>
       </c>
       <c r="H71" t="n">
         <v>3</v>
       </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3155,11 +3510,16 @@
         </is>
       </c>
       <c r="G72" t="n">
-        <v>53.07</v>
+        <v>53.48</v>
       </c>
       <c r="H72" t="n">
         <v>2</v>
       </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3193,11 +3553,16 @@
         </is>
       </c>
       <c r="G73" t="n">
-        <v>72.73</v>
+        <v>72.8</v>
       </c>
       <c r="H73" t="n">
         <v>4</v>
       </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3231,11 +3596,16 @@
         </is>
       </c>
       <c r="G74" t="n">
-        <v>72.26000000000001</v>
+        <v>72.39</v>
       </c>
       <c r="H74" t="n">
         <v>6</v>
       </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3269,11 +3639,16 @@
         </is>
       </c>
       <c r="G75" t="n">
-        <v>49.32</v>
+        <v>49.25</v>
       </c>
       <c r="H75" t="n">
         <v>19</v>
       </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3307,11 +3682,16 @@
         </is>
       </c>
       <c r="G76" t="n">
-        <v>27.61</v>
+        <v>26.96</v>
       </c>
       <c r="H76" t="n">
         <v>10</v>
       </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3345,11 +3725,16 @@
         </is>
       </c>
       <c r="G77" t="n">
-        <v>91.81999999999999</v>
+        <v>91.89</v>
       </c>
       <c r="H77" t="n">
         <v>19</v>
       </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3383,11 +3768,16 @@
         </is>
       </c>
       <c r="G78" t="n">
-        <v>37.02</v>
+        <v>36.87</v>
       </c>
       <c r="H78" t="n">
         <v>31</v>
       </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3421,11 +3811,16 @@
         </is>
       </c>
       <c r="G79" t="n">
-        <v>41.43</v>
+        <v>41.28</v>
       </c>
       <c r="H79" t="n">
         <v>9</v>
       </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3459,11 +3854,16 @@
         </is>
       </c>
       <c r="G80" t="n">
-        <v>70.63</v>
+        <v>70.56</v>
       </c>
       <c r="H80" t="n">
         <v>9</v>
       </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3497,11 +3897,16 @@
         </is>
       </c>
       <c r="G81" t="n">
-        <v>53.37</v>
+        <v>53.41</v>
       </c>
       <c r="H81" t="n">
         <v>12</v>
       </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3535,11 +3940,16 @@
         </is>
       </c>
       <c r="G82" t="n">
-        <v>52.81</v>
+        <v>53.18</v>
       </c>
       <c r="H82" t="n">
         <v>15</v>
       </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3573,11 +3983,16 @@
         </is>
       </c>
       <c r="G83" t="n">
-        <v>19.67</v>
+        <v>19.56</v>
       </c>
       <c r="H83" t="n">
         <v>15</v>
       </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3611,11 +4026,16 @@
         </is>
       </c>
       <c r="G84" t="n">
-        <v>4.7</v>
+        <v>4.75</v>
       </c>
       <c r="H84" t="n">
         <v>28</v>
       </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3649,11 +4069,16 @@
         </is>
       </c>
       <c r="G85" t="n">
-        <v>16.32</v>
+        <v>16.62</v>
       </c>
       <c r="H85" t="n">
         <v>36</v>
       </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>Steven Panagakos</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3687,11 +4112,16 @@
         </is>
       </c>
       <c r="G86" t="n">
-        <v>72.75</v>
+        <v>73.45</v>
       </c>
       <c r="H86" t="n">
         <v>4</v>
       </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3725,11 +4155,16 @@
         </is>
       </c>
       <c r="G87" t="n">
-        <v>31.88</v>
+        <v>32.35</v>
       </c>
       <c r="H87" t="n">
         <v>22</v>
       </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3763,11 +4198,16 @@
         </is>
       </c>
       <c r="G88" t="n">
-        <v>89.45</v>
+        <v>89.44</v>
       </c>
       <c r="H88" t="n">
         <v>4</v>
       </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3801,11 +4241,16 @@
         </is>
       </c>
       <c r="G89" t="n">
-        <v>0.84</v>
+        <v>0.85</v>
       </c>
       <c r="H89" t="n">
         <v>48</v>
       </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3839,11 +4284,16 @@
         </is>
       </c>
       <c r="G90" t="n">
-        <v>21.54</v>
+        <v>21.03</v>
       </c>
       <c r="H90" t="n">
         <v>16</v>
       </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3882,6 +4332,11 @@
       <c r="H91" t="n">
         <v>0</v>
       </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3915,11 +4370,16 @@
         </is>
       </c>
       <c r="G92" t="n">
-        <v>24.17</v>
+        <v>23.78</v>
       </c>
       <c r="H92" t="n">
         <v>30</v>
       </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3953,11 +4413,16 @@
         </is>
       </c>
       <c r="G93" t="n">
-        <v>94.04000000000001</v>
+        <v>94.06999999999999</v>
       </c>
       <c r="H93" t="n">
         <v>38</v>
       </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3991,11 +4456,16 @@
         </is>
       </c>
       <c r="G94" t="n">
-        <v>7.94</v>
+        <v>7.86</v>
       </c>
       <c r="H94" t="n">
         <v>71</v>
       </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4029,11 +4499,16 @@
         </is>
       </c>
       <c r="G95" t="n">
-        <v>55.6</v>
+        <v>55.7</v>
       </c>
       <c r="H95" t="n">
         <v>7</v>
       </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4067,11 +4542,16 @@
         </is>
       </c>
       <c r="G96" t="n">
-        <v>18.02</v>
+        <v>18.16</v>
       </c>
       <c r="H96" t="n">
         <v>67</v>
       </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4105,11 +4585,16 @@
         </is>
       </c>
       <c r="G97" t="n">
-        <v>27.59</v>
+        <v>27.39</v>
       </c>
       <c r="H97" t="n">
         <v>32</v>
       </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4143,11 +4628,16 @@
         </is>
       </c>
       <c r="G98" t="n">
-        <v>5.01</v>
+        <v>4.84</v>
       </c>
       <c r="H98" t="n">
         <v>64</v>
       </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4181,11 +4671,16 @@
         </is>
       </c>
       <c r="G99" t="n">
-        <v>63.9</v>
+        <v>64.64</v>
       </c>
       <c r="H99" t="n">
         <v>10</v>
       </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4219,11 +4714,16 @@
         </is>
       </c>
       <c r="G100" t="n">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
       <c r="H100" t="n">
         <v>76</v>
       </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4262,6 +4762,11 @@
       <c r="H101" t="n">
         <v>58</v>
       </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4295,11 +4800,16 @@
         </is>
       </c>
       <c r="G102" t="n">
-        <v>17.1</v>
+        <v>17.01</v>
       </c>
       <c r="H102" t="n">
         <v>39</v>
       </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>Matthew Coscia</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4333,11 +4843,16 @@
         </is>
       </c>
       <c r="G103" t="n">
-        <v>45.41</v>
+        <v>46.24</v>
       </c>
       <c r="H103" t="n">
         <v>30</v>
       </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4371,11 +4886,16 @@
         </is>
       </c>
       <c r="G104" t="n">
-        <v>73.06999999999999</v>
+        <v>73.72</v>
       </c>
       <c r="H104" t="n">
         <v>2</v>
       </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4409,11 +4929,16 @@
         </is>
       </c>
       <c r="G105" t="n">
-        <v>55.85</v>
+        <v>55.77</v>
       </c>
       <c r="H105" t="n">
         <v>8</v>
       </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -4447,11 +4972,16 @@
         </is>
       </c>
       <c r="G106" t="n">
-        <v>4.86</v>
+        <v>4.82</v>
       </c>
       <c r="H106" t="n">
         <v>43</v>
       </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4485,11 +5015,16 @@
         </is>
       </c>
       <c r="G107" t="n">
-        <v>14.95</v>
+        <v>15.07</v>
       </c>
       <c r="H107" t="n">
         <v>37</v>
       </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4523,11 +5058,16 @@
         </is>
       </c>
       <c r="G108" t="n">
-        <v>73.59</v>
+        <v>73.73999999999999</v>
       </c>
       <c r="H108" t="n">
         <v>27</v>
       </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4552,7 +5092,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>RB</t>
+          <t>BE</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -4561,11 +5101,16 @@
         </is>
       </c>
       <c r="G109" t="n">
-        <v>16.85</v>
+        <v>16.82</v>
       </c>
       <c r="H109" t="n">
         <v>26</v>
       </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4599,11 +5144,16 @@
         </is>
       </c>
       <c r="G110" t="n">
-        <v>7.42</v>
+        <v>7.41</v>
       </c>
       <c r="H110" t="n">
         <v>90</v>
       </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4637,11 +5187,16 @@
         </is>
       </c>
       <c r="G111" t="n">
-        <v>64.45999999999999</v>
+        <v>64.14</v>
       </c>
       <c r="H111" t="n">
         <v>23</v>
       </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4675,11 +5230,16 @@
         </is>
       </c>
       <c r="G112" t="n">
-        <v>18.78</v>
+        <v>18.66</v>
       </c>
       <c r="H112" t="n">
         <v>34</v>
       </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4713,11 +5273,16 @@
         </is>
       </c>
       <c r="G113" t="n">
-        <v>45.31</v>
+        <v>44.51</v>
       </c>
       <c r="H113" t="n">
         <v>9</v>
       </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -4751,11 +5316,16 @@
         </is>
       </c>
       <c r="G114" t="n">
-        <v>29.77</v>
+        <v>29.85</v>
       </c>
       <c r="H114" t="n">
         <v>5</v>
       </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4789,11 +5359,16 @@
         </is>
       </c>
       <c r="G115" t="n">
-        <v>12.42</v>
+        <v>12.09</v>
       </c>
       <c r="H115" t="n">
         <v>25</v>
       </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -4827,11 +5402,16 @@
         </is>
       </c>
       <c r="G116" t="n">
-        <v>66.70999999999999</v>
+        <v>66.47</v>
       </c>
       <c r="H116" t="n">
         <v>8</v>
       </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -4865,11 +5445,16 @@
         </is>
       </c>
       <c r="G117" t="n">
-        <v>14.63</v>
+        <v>14.7</v>
       </c>
       <c r="H117" t="n">
         <v>23</v>
       </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -4894,7 +5479,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>BE</t>
+          <t>RB</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -4903,11 +5488,16 @@
         </is>
       </c>
       <c r="G118" t="n">
-        <v>37.79</v>
+        <v>37.6</v>
       </c>
       <c r="H118" t="n">
         <v>32</v>
       </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -4941,11 +5531,16 @@
         </is>
       </c>
       <c r="G119" t="n">
-        <v>75.73</v>
+        <v>75.84</v>
       </c>
       <c r="H119" t="n">
         <v>25</v>
       </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>Chris Vanko</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -4979,11 +5574,16 @@
         </is>
       </c>
       <c r="G120" t="n">
-        <v>94.42</v>
+        <v>94.40000000000001</v>
       </c>
       <c r="H120" t="n">
         <v>1</v>
       </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>Braeden Twomey</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -5017,11 +5617,16 @@
         </is>
       </c>
       <c r="G121" t="n">
-        <v>79.40000000000001</v>
+        <v>79.38</v>
       </c>
       <c r="H121" t="n">
         <v>11</v>
       </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>Braeden Twomey</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -5055,11 +5660,16 @@
         </is>
       </c>
       <c r="G122" t="n">
-        <v>23.86</v>
+        <v>23.64</v>
       </c>
       <c r="H122" t="n">
         <v>17</v>
       </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>Braeden Twomey</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -5093,11 +5703,16 @@
         </is>
       </c>
       <c r="G123" t="n">
-        <v>27.78</v>
+        <v>27.12</v>
       </c>
       <c r="H123" t="n">
         <v>6</v>
       </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>Braeden Twomey</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -5131,11 +5746,16 @@
         </is>
       </c>
       <c r="G124" t="n">
-        <v>14.12</v>
+        <v>13.9</v>
       </c>
       <c r="H124" t="n">
         <v>66</v>
       </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>Braeden Twomey</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -5169,11 +5789,16 @@
         </is>
       </c>
       <c r="G125" t="n">
-        <v>66.48999999999999</v>
+        <v>67.09</v>
       </c>
       <c r="H125" t="n">
         <v>17</v>
       </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>Braeden Twomey</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -5207,11 +5832,16 @@
         </is>
       </c>
       <c r="G126" t="n">
-        <v>58.66</v>
+        <v>58.48</v>
       </c>
       <c r="H126" t="n">
         <v>54</v>
       </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>Braeden Twomey</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -5245,11 +5875,16 @@
         </is>
       </c>
       <c r="G127" t="n">
-        <v>46.18</v>
+        <v>45.98</v>
       </c>
       <c r="H127" t="n">
         <v>22</v>
       </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>Braeden Twomey</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -5283,11 +5918,16 @@
         </is>
       </c>
       <c r="G128" t="n">
-        <v>69.20999999999999</v>
+        <v>69.83</v>
       </c>
       <c r="H128" t="n">
         <v>13</v>
       </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>Braeden Twomey</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -5321,11 +5961,16 @@
         </is>
       </c>
       <c r="G129" t="n">
-        <v>10.94</v>
+        <v>11.09</v>
       </c>
       <c r="H129" t="n">
         <v>52</v>
       </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>Braeden Twomey</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -5359,11 +6004,16 @@
         </is>
       </c>
       <c r="G130" t="n">
-        <v>13.7</v>
+        <v>13.89</v>
       </c>
       <c r="H130" t="n">
         <v>17</v>
       </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>Braeden Twomey</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -5397,11 +6047,16 @@
         </is>
       </c>
       <c r="G131" t="n">
-        <v>7.38</v>
+        <v>7.25</v>
       </c>
       <c r="H131" t="n">
         <v>32</v>
       </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>Braeden Twomey</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -5435,11 +6090,16 @@
         </is>
       </c>
       <c r="G132" t="n">
-        <v>20.71</v>
+        <v>20.69</v>
       </c>
       <c r="H132" t="n">
         <v>23</v>
       </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>Braeden Twomey</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -5473,11 +6133,16 @@
         </is>
       </c>
       <c r="G133" t="n">
-        <v>6.99</v>
+        <v>7.01</v>
       </c>
       <c r="H133" t="n">
         <v>27</v>
       </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>Braeden Twomey</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -5511,11 +6176,16 @@
         </is>
       </c>
       <c r="G134" t="n">
-        <v>29.69</v>
+        <v>29.06</v>
       </c>
       <c r="H134" t="n">
         <v>10</v>
       </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>Braeden Twomey</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -5549,11 +6219,16 @@
         </is>
       </c>
       <c r="G135" t="n">
-        <v>74.52</v>
+        <v>75.13</v>
       </c>
       <c r="H135" t="n">
         <v>3</v>
       </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -5587,11 +6262,16 @@
         </is>
       </c>
       <c r="G136" t="n">
-        <v>62.42</v>
+        <v>63.11</v>
       </c>
       <c r="H136" t="n">
         <v>24</v>
       </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -5630,6 +6310,11 @@
       <c r="H137" t="n">
         <v>59</v>
       </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -5663,11 +6348,16 @@
         </is>
       </c>
       <c r="G138" t="n">
-        <v>82.43000000000001</v>
+        <v>82.45999999999999</v>
       </c>
       <c r="H138" t="n">
         <v>65</v>
       </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -5701,11 +6391,16 @@
         </is>
       </c>
       <c r="G139" t="n">
-        <v>17.25</v>
+        <v>17.16</v>
       </c>
       <c r="H139" t="n">
         <v>41</v>
       </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -5744,6 +6439,11 @@
       <c r="H140" t="n">
         <v>51</v>
       </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -5777,11 +6477,16 @@
         </is>
       </c>
       <c r="G141" t="n">
-        <v>84.73999999999999</v>
+        <v>84.77</v>
       </c>
       <c r="H141" t="n">
         <v>5</v>
       </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -5820,6 +6525,11 @@
       <c r="H142" t="n">
         <v>77</v>
       </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -5853,11 +6563,16 @@
         </is>
       </c>
       <c r="G143" t="n">
-        <v>69.84999999999999</v>
+        <v>69.70999999999999</v>
       </c>
       <c r="H143" t="n">
         <v>1</v>
       </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -5896,6 +6611,11 @@
       <c r="H144" t="n">
         <v>4</v>
       </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -5929,11 +6649,16 @@
         </is>
       </c>
       <c r="G145" t="n">
-        <v>86.04000000000001</v>
+        <v>86.05</v>
       </c>
       <c r="H145" t="n">
         <v>17</v>
       </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -5972,6 +6697,11 @@
       <c r="H146" t="n">
         <v>140</v>
       </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -6005,11 +6735,16 @@
         </is>
       </c>
       <c r="G147" t="n">
-        <v>71.45</v>
+        <v>71.8</v>
       </c>
       <c r="H147" t="n">
         <v>41</v>
       </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -6043,11 +6778,16 @@
         </is>
       </c>
       <c r="G148" t="n">
-        <v>1.66</v>
+        <v>1.62</v>
       </c>
       <c r="H148" t="n">
         <v>43</v>
       </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -6081,11 +6821,16 @@
         </is>
       </c>
       <c r="G149" t="n">
-        <v>25.16</v>
+        <v>25.69</v>
       </c>
       <c r="H149" t="n">
         <v>59</v>
       </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -6124,6 +6869,11 @@
       <c r="H150" t="n">
         <v>45</v>
       </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -6157,11 +6907,16 @@
         </is>
       </c>
       <c r="G151" t="n">
-        <v>18.46</v>
+        <v>18.76</v>
       </c>
       <c r="H151" t="n">
         <v>8</v>
       </c>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>Justin Gaines</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -6200,6 +6955,11 @@
       <c r="H152" t="n">
         <v>2</v>
       </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -6233,11 +6993,16 @@
         </is>
       </c>
       <c r="G153" t="n">
-        <v>91.76000000000001</v>
+        <v>91.81999999999999</v>
       </c>
       <c r="H153" t="n">
         <v>7</v>
       </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -6271,11 +7036,16 @@
         </is>
       </c>
       <c r="G154" t="n">
-        <v>39.22</v>
+        <v>38.58</v>
       </c>
       <c r="H154" t="n">
         <v>9</v>
       </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -6309,11 +7079,16 @@
         </is>
       </c>
       <c r="G155" t="n">
-        <v>53.65</v>
+        <v>54.16</v>
       </c>
       <c r="H155" t="n">
         <v>13</v>
       </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -6347,11 +7122,16 @@
         </is>
       </c>
       <c r="G156" t="n">
-        <v>26.58</v>
+        <v>26.3</v>
       </c>
       <c r="H156" t="n">
         <v>29</v>
       </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -6385,11 +7165,16 @@
         </is>
       </c>
       <c r="G157" t="n">
-        <v>69.48</v>
+        <v>69.59</v>
       </c>
       <c r="H157" t="n">
         <v>6</v>
       </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -6423,11 +7208,16 @@
         </is>
       </c>
       <c r="G158" t="n">
-        <v>80.64</v>
+        <v>80.48</v>
       </c>
       <c r="H158" t="n">
         <v>1</v>
       </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -6461,11 +7251,16 @@
         </is>
       </c>
       <c r="G159" t="n">
-        <v>6.6</v>
+        <v>6.5</v>
       </c>
       <c r="H159" t="n">
         <v>31</v>
       </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -6499,11 +7294,16 @@
         </is>
       </c>
       <c r="G160" t="n">
-        <v>81.48</v>
+        <v>81.45999999999999</v>
       </c>
       <c r="H160" t="n">
         <v>13</v>
       </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -6537,11 +7337,16 @@
         </is>
       </c>
       <c r="G161" t="n">
-        <v>64.67</v>
+        <v>65.27</v>
       </c>
       <c r="H161" t="n">
         <v>7</v>
       </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -6575,11 +7380,16 @@
         </is>
       </c>
       <c r="G162" t="n">
-        <v>67.56999999999999</v>
+        <v>67.41</v>
       </c>
       <c r="H162" t="n">
         <v>11</v>
       </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -6613,11 +7423,16 @@
         </is>
       </c>
       <c r="G163" t="n">
-        <v>32.09</v>
+        <v>31.88</v>
       </c>
       <c r="H163" t="n">
         <v>25</v>
       </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -6651,11 +7466,16 @@
         </is>
       </c>
       <c r="G164" t="n">
-        <v>26.05</v>
+        <v>25.58</v>
       </c>
       <c r="H164" t="n">
         <v>37</v>
       </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -6689,11 +7509,16 @@
         </is>
       </c>
       <c r="G165" t="n">
-        <v>73.43000000000001</v>
+        <v>73.38</v>
       </c>
       <c r="H165" t="n">
         <v>34</v>
       </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -6727,11 +7552,16 @@
         </is>
       </c>
       <c r="G166" t="n">
-        <v>43.11</v>
+        <v>43.59</v>
       </c>
       <c r="H166" t="n">
         <v>22</v>
       </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -6770,6 +7600,11 @@
       <c r="H167" t="n">
         <v>17</v>
       </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>Jackson Noto</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -6808,6 +7643,11 @@
       <c r="H168" t="n">
         <v>1</v>
       </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -6841,11 +7681,16 @@
         </is>
       </c>
       <c r="G169" t="n">
-        <v>13.85</v>
+        <v>13.83</v>
       </c>
       <c r="H169" t="n">
         <v>20</v>
       </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -6879,11 +7724,16 @@
         </is>
       </c>
       <c r="G170" t="n">
-        <v>50.64</v>
+        <v>50.58</v>
       </c>
       <c r="H170" t="n">
         <v>22</v>
       </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -6917,11 +7767,16 @@
         </is>
       </c>
       <c r="G171" t="n">
-        <v>10.18</v>
+        <v>10.42</v>
       </c>
       <c r="H171" t="n">
         <v>47</v>
       </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -6955,11 +7810,16 @@
         </is>
       </c>
       <c r="G172" t="n">
-        <v>24.48</v>
+        <v>24.72</v>
       </c>
       <c r="H172" t="n">
         <v>28</v>
       </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -6993,11 +7853,16 @@
         </is>
       </c>
       <c r="G173" t="n">
-        <v>39.83</v>
+        <v>39.78</v>
       </c>
       <c r="H173" t="n">
         <v>12</v>
       </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -7031,11 +7896,16 @@
         </is>
       </c>
       <c r="G174" t="n">
-        <v>80.23</v>
+        <v>80.33</v>
       </c>
       <c r="H174" t="n">
         <v>4</v>
       </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -7069,11 +7939,16 @@
         </is>
       </c>
       <c r="G175" t="n">
-        <v>34.08</v>
+        <v>33.96</v>
       </c>
       <c r="H175" t="n">
         <v>8</v>
       </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -7107,11 +7982,16 @@
         </is>
       </c>
       <c r="G176" t="n">
-        <v>68.55</v>
+        <v>68.45999999999999</v>
       </c>
       <c r="H176" t="n">
         <v>8</v>
       </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -7145,11 +8025,16 @@
         </is>
       </c>
       <c r="G177" t="n">
-        <v>15.34</v>
+        <v>15.24</v>
       </c>
       <c r="H177" t="n">
         <v>44</v>
       </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -7183,11 +8068,16 @@
         </is>
       </c>
       <c r="G178" t="n">
-        <v>88.59999999999999</v>
+        <v>88.54000000000001</v>
       </c>
       <c r="H178" t="n">
         <v>15</v>
       </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -7221,11 +8111,16 @@
         </is>
       </c>
       <c r="G179" t="n">
-        <v>58.05</v>
+        <v>57.91</v>
       </c>
       <c r="H179" t="n">
         <v>15</v>
       </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -7259,11 +8154,16 @@
         </is>
       </c>
       <c r="G180" t="n">
-        <v>13.62</v>
+        <v>13.61</v>
       </c>
       <c r="H180" t="n">
         <v>11</v>
       </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -7297,11 +8197,16 @@
         </is>
       </c>
       <c r="G181" t="n">
-        <v>5.36</v>
+        <v>5.3</v>
       </c>
       <c r="H181" t="n">
         <v>40</v>
       </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -7335,11 +8240,16 @@
         </is>
       </c>
       <c r="G182" t="n">
-        <v>17.14</v>
+        <v>16.94</v>
       </c>
       <c r="H182" t="n">
         <v>23</v>
       </c>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -7373,11 +8283,16 @@
         </is>
       </c>
       <c r="G183" t="n">
-        <v>71.67</v>
+        <v>71.79000000000001</v>
       </c>
       <c r="H183" t="n">
         <v>34</v>
       </c>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>Matt Murawski</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -7411,11 +8326,16 @@
         </is>
       </c>
       <c r="G184" t="n">
-        <v>58.2</v>
+        <v>58.81</v>
       </c>
       <c r="H184" t="n">
         <v>5</v>
       </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -7449,11 +8369,16 @@
         </is>
       </c>
       <c r="G185" t="n">
-        <v>53.55</v>
+        <v>53.97</v>
       </c>
       <c r="H185" t="n">
         <v>36</v>
       </c>
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -7487,11 +8412,16 @@
         </is>
       </c>
       <c r="G186" t="n">
-        <v>82.84</v>
+        <v>82.81</v>
       </c>
       <c r="H186" t="n">
         <v>3</v>
       </c>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -7525,11 +8455,16 @@
         </is>
       </c>
       <c r="G187" t="n">
-        <v>49.13</v>
+        <v>48.96</v>
       </c>
       <c r="H187" t="n">
         <v>26</v>
       </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -7563,11 +8498,16 @@
         </is>
       </c>
       <c r="G188" t="n">
-        <v>59.48</v>
+        <v>59.55</v>
       </c>
       <c r="H188" t="n">
         <v>3</v>
       </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -7606,6 +8546,11 @@
       <c r="H189" t="n">
         <v>0</v>
       </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -7639,11 +8584,16 @@
         </is>
       </c>
       <c r="G190" t="n">
-        <v>8.949999999999999</v>
+        <v>8.779999999999999</v>
       </c>
       <c r="H190" t="n">
         <v>6</v>
       </c>
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -7677,11 +8627,16 @@
         </is>
       </c>
       <c r="G191" t="n">
-        <v>49.72</v>
+        <v>49.49</v>
       </c>
       <c r="H191" t="n">
         <v>14</v>
       </c>
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -7715,11 +8670,16 @@
         </is>
       </c>
       <c r="G192" t="n">
-        <v>3.44</v>
+        <v>3.36</v>
       </c>
       <c r="H192" t="n">
         <v>20</v>
       </c>
+      <c r="I192" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -7753,11 +8713,16 @@
         </is>
       </c>
       <c r="G193" t="n">
-        <v>11.34</v>
+        <v>11.33</v>
       </c>
       <c r="H193" t="n">
         <v>33</v>
       </c>
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -7791,11 +8756,16 @@
         </is>
       </c>
       <c r="G194" t="n">
-        <v>4.52</v>
+        <v>4.54</v>
       </c>
       <c r="H194" t="n">
         <v>132</v>
       </c>
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -7829,11 +8799,16 @@
         </is>
       </c>
       <c r="G195" t="n">
-        <v>0.73</v>
+        <v>0.71</v>
       </c>
       <c r="H195" t="n">
         <v>47</v>
       </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -7867,11 +8842,16 @@
         </is>
       </c>
       <c r="G196" t="n">
-        <v>40.99</v>
+        <v>41.59</v>
       </c>
       <c r="H196" t="n">
         <v>46</v>
       </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -7905,11 +8885,16 @@
         </is>
       </c>
       <c r="G197" t="n">
-        <v>22.99</v>
+        <v>22.89</v>
       </c>
       <c r="H197" t="n">
         <v>35</v>
       </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -7943,11 +8928,16 @@
         </is>
       </c>
       <c r="G198" t="n">
-        <v>34.57</v>
+        <v>35.3</v>
       </c>
       <c r="H198" t="n">
         <v>13</v>
       </c>
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -7981,11 +8971,16 @@
         </is>
       </c>
       <c r="G199" t="n">
-        <v>3.62</v>
+        <v>3.69</v>
       </c>
       <c r="H199" t="n">
         <v>18</v>
       </c>
+      <c r="I199" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -8019,10 +9014,15 @@
         </is>
       </c>
       <c r="G200" t="n">
-        <v>53.4</v>
+        <v>53.97</v>
       </c>
       <c r="H200" t="n">
         <v>23</v>
+      </c>
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>Alex Dodson</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>